<commit_message>
fix Profile Duration.ms > Duration.INT.ms
</commit_message>
<xml_diff>
--- a/MEC_Meter/doku/IPS-Modul PowerMeter DataPoints.xlsx
+++ b/MEC_Meter/doku/IPS-Modul PowerMeter DataPoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud\ownCube\SmartHome\Hardware\Smart Meter - Verbund (Flexiciency)\Doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5A685E-728A-40B9-8EE3-0D0D296914F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C57973E-27FC-4904-83B6-F2D041F57BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25830" yWindow="345" windowWidth="24255" windowHeight="22530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1526,9 +1526,6 @@
     <t>Operating Time (last fctory reset)</t>
   </si>
   <si>
-    <t>Duration.ms</t>
-  </si>
-  <si>
     <t>Apparent Forward Energy - Phase A</t>
   </si>
   <si>
@@ -1728,6 +1725,9 @@
   </si>
   <si>
     <t>false</t>
+  </si>
+  <si>
+    <t>Duration.INT.ms</t>
   </si>
 </sst>
 </file>
@@ -2152,7 +2152,7 @@
   <dimension ref="A1:M130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2330,7 +2330,7 @@
         <v>299</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>495</v>
+        <v>562</v>
       </c>
       <c r="E5" s="4">
         <v>1</v>
@@ -2355,7 +2355,7 @@
       </c>
       <c r="M5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>'TIME' =&gt; ['Operating Time (last fctory reset)', VARIABLETYPE_INTEGER, 'Duration.ms', 1, 0, 'Basic', 'Basic', 10, 4, true],</v>
+        <v>'TIME' =&gt; ['Operating Time (last fctory reset)', VARIABLETYPE_INTEGER, 'Duration.INT.ms', 1, 0, 'Basic', 'Basic', 10, 4, true],</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2725,7 +2725,7 @@
         <v>2</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H15" s="21" t="s">
         <v>296</v>
@@ -2737,7 +2737,7 @@
         <v>14</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="M15" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2762,7 +2762,7 @@
         <v>2</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H16" s="21" t="s">
         <v>296</v>
@@ -2774,7 +2774,7 @@
         <v>15</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="M16" s="3" t="str">
         <f t="shared" si="0"/>
@@ -3059,7 +3059,7 @@
         <v>89</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>298</v>
@@ -3215,7 +3215,7 @@
         <v>88</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>298</v>
@@ -3449,7 +3449,7 @@
         <v>252</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>298</v>
@@ -3464,10 +3464,10 @@
         <v>3</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I34" s="7">
         <v>36</v>
@@ -3488,7 +3488,7 @@
         <v>253</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>298</v>
@@ -3503,10 +3503,10 @@
         <v>3</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I35" s="7">
         <v>36</v>
@@ -3527,7 +3527,7 @@
         <v>254</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>298</v>
@@ -3542,10 +3542,10 @@
         <v>3</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I36" s="7">
         <v>36</v>
@@ -3944,7 +3944,7 @@
         <v>38</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>298</v>
@@ -3959,10 +3959,10 @@
         <v>2</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I47" s="7">
         <v>60</v>
@@ -3983,7 +3983,7 @@
         <v>39</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>298</v>
@@ -3998,10 +3998,10 @@
         <v>2</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I48" s="7">
         <v>60</v>
@@ -4022,7 +4022,7 @@
         <v>40</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>298</v>
@@ -4037,10 +4037,10 @@
         <v>2</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I49" s="7">
         <v>60</v>
@@ -4061,7 +4061,7 @@
         <v>41</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>298</v>
@@ -4076,10 +4076,10 @@
         <v>2</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I50" s="7">
         <v>60</v>
@@ -4100,7 +4100,7 @@
         <v>62</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>298</v>
@@ -4115,10 +4115,10 @@
         <v>3</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I51" s="7">
         <v>65</v>
@@ -4139,7 +4139,7 @@
         <v>63</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>298</v>
@@ -4154,10 +4154,10 @@
         <v>3</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I52" s="7">
         <v>65</v>
@@ -4178,7 +4178,7 @@
         <v>64</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>298</v>
@@ -4193,10 +4193,10 @@
         <v>3</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I53" s="7">
         <v>65</v>
@@ -4217,7 +4217,7 @@
         <v>65</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>298</v>
@@ -4232,10 +4232,10 @@
         <v>3</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I54" s="7">
         <v>65</v>
@@ -4271,10 +4271,10 @@
         <v>3</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I55" s="7">
         <v>65</v>
@@ -4310,10 +4310,10 @@
         <v>3</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I56" s="7">
         <v>65</v>
@@ -4349,10 +4349,10 @@
         <v>3</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I57" s="7">
         <v>65</v>
@@ -4388,10 +4388,10 @@
         <v>3</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I58" s="7">
         <v>65</v>
@@ -4412,7 +4412,7 @@
         <v>235</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>298</v>
@@ -4427,10 +4427,10 @@
         <v>3</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I59" s="7">
         <v>66</v>
@@ -4451,7 +4451,7 @@
         <v>236</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>298</v>
@@ -4466,10 +4466,10 @@
         <v>3</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I60" s="7">
         <v>66</v>
@@ -4490,7 +4490,7 @@
         <v>237</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>298</v>
@@ -4505,10 +4505,10 @@
         <v>3</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I61" s="7">
         <v>66</v>
@@ -4529,7 +4529,7 @@
         <v>238</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>298</v>
@@ -4544,10 +4544,10 @@
         <v>3</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I62" s="7">
         <v>66</v>
@@ -4568,7 +4568,7 @@
         <v>239</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>298</v>
@@ -4583,10 +4583,10 @@
         <v>3</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I63" s="7">
         <v>66</v>
@@ -4607,7 +4607,7 @@
         <v>240</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>298</v>
@@ -4622,10 +4622,10 @@
         <v>3</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I64" s="7">
         <v>66</v>
@@ -4646,7 +4646,7 @@
         <v>241</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>298</v>
@@ -4661,10 +4661,10 @@
         <v>3</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I65" s="7">
         <v>66</v>
@@ -4685,7 +4685,7 @@
         <v>242</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>298</v>
@@ -4700,10 +4700,10 @@
         <v>3</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I66" s="7">
         <v>66</v>
@@ -4724,7 +4724,7 @@
         <v>243</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>298</v>
@@ -4739,10 +4739,10 @@
         <v>3</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I67" s="7">
         <v>66</v>
@@ -4763,7 +4763,7 @@
         <v>244</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>298</v>
@@ -4778,10 +4778,10 @@
         <v>3</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I68" s="7">
         <v>66</v>
@@ -4802,7 +4802,7 @@
         <v>245</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>298</v>
@@ -4817,10 +4817,10 @@
         <v>3</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I69" s="7">
         <v>66</v>
@@ -4841,7 +4841,7 @@
         <v>246</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>298</v>
@@ -4856,10 +4856,10 @@
         <v>3</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I70" s="7">
         <v>66</v>
@@ -4880,7 +4880,7 @@
         <v>247</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C71" s="6" t="s">
         <v>298</v>
@@ -4895,10 +4895,10 @@
         <v>3</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I71" s="7">
         <v>66</v>
@@ -4919,7 +4919,7 @@
         <v>248</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>298</v>
@@ -4934,10 +4934,10 @@
         <v>3</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I72" s="7">
         <v>66</v>
@@ -4958,7 +4958,7 @@
         <v>249</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>298</v>
@@ -4973,10 +4973,10 @@
         <v>3</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I73" s="7">
         <v>66</v>
@@ -4997,7 +4997,7 @@
         <v>250</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>298</v>
@@ -5012,10 +5012,10 @@
         <v>3</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I74" s="7">
         <v>66</v>
@@ -5036,7 +5036,7 @@
         <v>42</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>298</v>
@@ -5051,10 +5051,10 @@
         <v>2</v>
       </c>
       <c r="G75" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I75" s="7">
         <v>70</v>
@@ -5075,7 +5075,7 @@
         <v>43</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>298</v>
@@ -5090,10 +5090,10 @@
         <v>2</v>
       </c>
       <c r="G76" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I76" s="7">
         <v>70</v>
@@ -5114,7 +5114,7 @@
         <v>44</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>298</v>
@@ -5129,10 +5129,10 @@
         <v>2</v>
       </c>
       <c r="G77" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I77" s="7">
         <v>70</v>
@@ -5153,7 +5153,7 @@
         <v>45</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>298</v>
@@ -5168,10 +5168,10 @@
         <v>2</v>
       </c>
       <c r="G78" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I78" s="7">
         <v>70</v>
@@ -5192,7 +5192,7 @@
         <v>226</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>298</v>
@@ -5207,10 +5207,10 @@
         <v>2</v>
       </c>
       <c r="G79" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I79" s="7">
         <v>70</v>
@@ -5231,7 +5231,7 @@
         <v>82</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>298</v>
@@ -5246,10 +5246,10 @@
         <v>3</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I80" s="7">
         <v>75</v>
@@ -5270,7 +5270,7 @@
         <v>83</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>298</v>
@@ -5285,10 +5285,10 @@
         <v>3</v>
       </c>
       <c r="G81" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I81" s="7">
         <v>75</v>
@@ -5309,7 +5309,7 @@
         <v>84</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>298</v>
@@ -5324,10 +5324,10 @@
         <v>3</v>
       </c>
       <c r="G82" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I82" s="7">
         <v>75</v>
@@ -5348,7 +5348,7 @@
         <v>85</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>298</v>
@@ -5363,10 +5363,10 @@
         <v>3</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I83" s="7">
         <v>75</v>
@@ -5387,7 +5387,7 @@
         <v>225</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>298</v>
@@ -5402,10 +5402,10 @@
         <v>3</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I84" s="7">
         <v>75</v>
@@ -5441,10 +5441,10 @@
         <v>3</v>
       </c>
       <c r="G85" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I85" s="7">
         <v>75</v>
@@ -5480,10 +5480,10 @@
         <v>3</v>
       </c>
       <c r="G86" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I86" s="7">
         <v>75</v>
@@ -5519,10 +5519,10 @@
         <v>3</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I87" s="7">
         <v>75</v>
@@ -5558,10 +5558,10 @@
         <v>3</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I88" s="7">
         <v>75</v>
@@ -5582,7 +5582,7 @@
         <v>231</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>298</v>
@@ -5597,10 +5597,10 @@
         <v>3</v>
       </c>
       <c r="G89" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I89" s="7">
         <v>75</v>
@@ -5621,7 +5621,7 @@
         <v>232</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>298</v>
@@ -5636,10 +5636,10 @@
         <v>3</v>
       </c>
       <c r="G90" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I90" s="7">
         <v>75</v>
@@ -5660,7 +5660,7 @@
         <v>233</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>298</v>
@@ -5675,10 +5675,10 @@
         <v>3</v>
       </c>
       <c r="G91" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I91" s="7">
         <v>75</v>
@@ -5699,7 +5699,7 @@
         <v>234</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>298</v>
@@ -5714,10 +5714,10 @@
         <v>3</v>
       </c>
       <c r="G92" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I92" s="7">
         <v>75</v>
@@ -5753,10 +5753,10 @@
         <v>2</v>
       </c>
       <c r="G93" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="H93" s="3" t="s">
         <v>559</v>
-      </c>
-      <c r="H93" s="3" t="s">
-        <v>560</v>
       </c>
       <c r="I93" s="7">
         <v>80</v>
@@ -5792,10 +5792,10 @@
         <v>2</v>
       </c>
       <c r="G94" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="H94" s="3" t="s">
         <v>559</v>
-      </c>
-      <c r="H94" s="3" t="s">
-        <v>560</v>
       </c>
       <c r="I94" s="7">
         <v>80</v>
@@ -5831,10 +5831,10 @@
         <v>2</v>
       </c>
       <c r="G95" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="H95" s="3" t="s">
         <v>559</v>
-      </c>
-      <c r="H95" s="3" t="s">
-        <v>560</v>
       </c>
       <c r="I95" s="7">
         <v>80</v>
@@ -5870,10 +5870,10 @@
         <v>2</v>
       </c>
       <c r="G96" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="H96" s="3" t="s">
         <v>559</v>
-      </c>
-      <c r="H96" s="3" t="s">
-        <v>560</v>
       </c>
       <c r="I96" s="7">
         <v>80</v>
@@ -5909,10 +5909,10 @@
         <v>2</v>
       </c>
       <c r="G97" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="H97" s="3" t="s">
         <v>559</v>
-      </c>
-      <c r="H97" s="3" t="s">
-        <v>560</v>
       </c>
       <c r="I97" s="7">
         <v>80</v>
@@ -5948,10 +5948,10 @@
         <v>2</v>
       </c>
       <c r="G98" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="H98" s="3" t="s">
         <v>559</v>
-      </c>
-      <c r="H98" s="3" t="s">
-        <v>560</v>
       </c>
       <c r="I98" s="7">
         <v>80</v>
@@ -5987,10 +5987,10 @@
         <v>2</v>
       </c>
       <c r="G99" s="7" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I99" s="7">
         <v>90</v>
@@ -6026,10 +6026,10 @@
         <v>2</v>
       </c>
       <c r="G100" s="7" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I100" s="7">
         <v>90</v>
@@ -6065,10 +6065,10 @@
         <v>2</v>
       </c>
       <c r="G101" s="7" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I101" s="7">
         <v>90</v>
@@ -6104,10 +6104,10 @@
         <v>2</v>
       </c>
       <c r="G102" s="7" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I102" s="7">
         <v>90</v>
@@ -6143,10 +6143,10 @@
         <v>3</v>
       </c>
       <c r="G103" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I103" s="7">
         <v>91</v>
@@ -6182,10 +6182,10 @@
         <v>3</v>
       </c>
       <c r="G104" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I104" s="7">
         <v>91</v>
@@ -6221,10 +6221,10 @@
         <v>3</v>
       </c>
       <c r="G105" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I105" s="7">
         <v>91</v>
@@ -6260,10 +6260,10 @@
         <v>3</v>
       </c>
       <c r="G106" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I106" s="7">
         <v>91</v>
@@ -6299,10 +6299,10 @@
         <v>3</v>
       </c>
       <c r="G107" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I107" s="7">
         <v>91</v>
@@ -6338,10 +6338,10 @@
         <v>3</v>
       </c>
       <c r="G108" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I108" s="7">
         <v>91</v>
@@ -6377,10 +6377,10 @@
         <v>3</v>
       </c>
       <c r="G109" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I109" s="7">
         <v>91</v>
@@ -6416,10 +6416,10 @@
         <v>3</v>
       </c>
       <c r="G110" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I110" s="7">
         <v>91</v>
@@ -6455,10 +6455,10 @@
         <v>2</v>
       </c>
       <c r="G111" s="7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H111" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I111" s="7">
         <v>95</v>
@@ -6494,10 +6494,10 @@
         <v>2</v>
       </c>
       <c r="G112" s="7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H112" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I112" s="7">
         <v>95</v>
@@ -6533,10 +6533,10 @@
         <v>2</v>
       </c>
       <c r="G113" s="7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I113" s="7">
         <v>95</v>
@@ -6572,10 +6572,10 @@
         <v>2</v>
       </c>
       <c r="G114" s="7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H114" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I114" s="7">
         <v>95</v>
@@ -6611,10 +6611,10 @@
         <v>3</v>
       </c>
       <c r="G115" s="7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I115" s="7">
         <v>96</v>
@@ -6650,10 +6650,10 @@
         <v>3</v>
       </c>
       <c r="G116" s="7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H116" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I116" s="7">
         <v>96</v>
@@ -6689,10 +6689,10 @@
         <v>3</v>
       </c>
       <c r="G117" s="7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H117" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I117" s="7">
         <v>96</v>
@@ -6728,10 +6728,10 @@
         <v>3</v>
       </c>
       <c r="G118" s="7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H118" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I118" s="7">
         <v>96</v>
@@ -6767,10 +6767,10 @@
         <v>3</v>
       </c>
       <c r="G119" s="7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H119" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I119" s="7">
         <v>96</v>
@@ -6806,10 +6806,10 @@
         <v>3</v>
       </c>
       <c r="G120" s="7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H120" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I120" s="7">
         <v>96</v>
@@ -6845,10 +6845,10 @@
         <v>3</v>
       </c>
       <c r="G121" s="7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H121" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I121" s="7">
         <v>96</v>
@@ -6885,10 +6885,10 @@
         <v>3</v>
       </c>
       <c r="G122" s="7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H122" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I122" s="7">
         <v>96</v>

</xml_diff>